<commit_message>
Added cycles to name + Added cycle save
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dokumente\!dhbw\6. semester\Flowchart-RealtimeSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C30EDE67-ADD1-4D18-B71A-5839820D32E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8193BE58-647A-41E7-ABDA-E986728FD22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17865" yWindow="3660" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -462,7 +462,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -540,7 +540,7 @@
         <v>13</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -569,7 +569,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -598,7 +598,7 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>

</xml_diff>

<commit_message>
Added simple mutex logic
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Dokumente\!dhbw\6. semester\Flowchart-RealtimeSystems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8193BE58-647A-41E7-ABDA-E986728FD22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55500AFC-46C2-412A-808F-BB1423314629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17865" yWindow="3660" windowWidth="16410" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>TASK</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>INITIAL_VALUE</t>
+  </si>
+  <si>
+    <t>MUTEX_LIST</t>
+  </si>
+  <si>
+    <t>m1</t>
   </si>
 </sst>
 </file>
@@ -459,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,21 +492,24 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -519,20 +528,23 @@
       <c r="F2">
         <v>159</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>15</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -551,20 +563,20 @@
       <c r="F3">
         <v>163</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>16</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>15</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -580,20 +592,23 @@
       <c r="F4">
         <v>426</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
         <v>15</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -609,16 +624,19 @@
       <c r="F5">
         <v>781</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>12</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bugfix mutex stays unlocked and error ppear
</commit_message>
<xml_diff>
--- a/data2.xlsx
+++ b/data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Marvin\Documents\Studium\Echtzeitsysteme\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED21DEFA-2C7A-4FA8-841B-E15F84A3E450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA112D15-F1B9-4F0D-A099-30744F95B5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,7 +454,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +527,7 @@
         <v>16</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>16</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>